<commit_message>
add rideshare, car-ev-phv, car-ev-phv-re, loss, insrenov and clothes-home
</commit_message>
<xml_diff>
--- a/src/tests/option-carshare.test-cases.xlsx
+++ b/src/tests/option-carshare.test-cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naoto/Documents/projects/code-for-japan/JibungotoPlanet-backend/src/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7B3298-C65F-2543-A7A2-659AF6D22614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64EEC9E1-AE75-EC41-A7E0-011C534AD235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6700" yWindow="3260" windowWidth="41860" windowHeight="19760" activeTab="1" xr2:uid="{504EB999-7D82-6E4A-B2A0-71B74C50F3FE}"/>
+    <workbookView xWindow="6700" yWindow="3260" windowWidth="41860" windowHeight="19760" xr2:uid="{504EB999-7D82-6E4A-B2A0-71B74C50F3FE}"/>
   </bookViews>
   <sheets>
     <sheet name="answers" sheetId="24" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="114">
   <si>
     <t>case</t>
     <phoneticPr fontId="1"/>
@@ -307,10 +307,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>carPassengersKey</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>privateCarAnnualMileage</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -360,10 +356,6 @@
   </si>
   <si>
     <t>motorbikeWeeklyTravelingTime</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>1_private-car-factor</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -597,6 +589,10 @@
       <t>ゾウゲン</t>
     </rPh>
     <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>carPassengersFirstKey</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -1067,6 +1063,12 @@
     <xf numFmtId="176" fontId="10" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="12" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="12" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="12" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="12" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="12" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1076,12 +1078,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="12" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="12" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="12" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="12" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="12" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="パーセント" xfId="1" builtinId="5"/>
@@ -2330,8 +2326,8 @@
   </sheetPr>
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -2361,7 +2357,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="18" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>55</v>
@@ -2373,21 +2369,21 @@
         <v>1</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>16</v>
@@ -2395,7 +2391,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>54</v>
@@ -2412,16 +2408,16 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>72</v>
+        <v>113</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>16</v>
@@ -2429,13 +2425,13 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D6" s="1">
         <v>5000</v>
@@ -2446,13 +2442,13 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D7" s="1">
         <v>5</v>
@@ -2463,13 +2459,13 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
@@ -2480,13 +2476,13 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
@@ -2497,13 +2493,13 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
@@ -2514,30 +2510,30 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D11" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>52</v>
@@ -2548,13 +2544,13 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D13" s="1">
         <v>20</v>
@@ -2565,13 +2561,13 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D14" s="1">
         <v>20</v>
@@ -2582,13 +2578,13 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D15" s="1">
         <v>20</v>
@@ -2599,13 +2595,13 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D16" s="1">
         <v>2</v>
@@ -2616,13 +2612,13 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D17" s="1">
         <v>20</v>
@@ -2633,13 +2629,13 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D18" s="2">
         <v>3</v>
@@ -2662,7 +2658,7 @@
   </sheetPr>
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -2717,23 +2713,23 @@
       <c r="K1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="40" t="s">
-        <v>101</v>
-      </c>
-      <c r="M1" s="41"/>
-      <c r="N1" s="42"/>
+      <c r="L1" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="M1" s="47"/>
+      <c r="N1" s="48"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D2" s="43">
+        <v>73</v>
+      </c>
+      <c r="D2" s="40">
         <v>12000</v>
       </c>
       <c r="E2" s="4" t="s">
@@ -2763,15 +2759,15 @@
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D3" s="44">
+        <v>74</v>
+      </c>
+      <c r="D3" s="41">
         <v>16700</v>
       </c>
       <c r="E3" s="8" t="s">
@@ -2801,15 +2797,15 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="D4" s="44">
+        <v>75</v>
+      </c>
+      <c r="D4" s="41">
         <v>1490</v>
       </c>
       <c r="E4" s="8" t="s">
@@ -2839,15 +2835,15 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" s="44">
+        <v>76</v>
+      </c>
+      <c r="D5" s="41">
         <v>120</v>
       </c>
       <c r="E5" s="8" t="s">
@@ -2877,15 +2873,15 @@
     </row>
     <row r="6" spans="1:14" ht="21" thickBot="1">
       <c r="A6" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" s="44">
+        <v>77</v>
+      </c>
+      <c r="D6" s="41">
         <v>1072.0879061735334</v>
       </c>
       <c r="E6" s="8" t="s">
@@ -2911,21 +2907,21 @@
       </c>
       <c r="L6" s="35"/>
       <c r="M6" s="29" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N6" s="30"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D7" s="45">
+        <v>78</v>
+      </c>
+      <c r="D7" s="42">
         <v>0</v>
       </c>
       <c r="E7" s="8" t="s">
@@ -2950,7 +2946,7 @@
         <v>35</v>
       </c>
       <c r="L7" s="31" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M7" s="19">
         <v>5000</v>
@@ -2961,15 +2957,15 @@
     </row>
     <row r="8" spans="1:14" ht="21" thickBot="1">
       <c r="A8" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="D8" s="46">
+        <v>77</v>
+      </c>
+      <c r="D8" s="43">
         <v>6352.9120938264668</v>
       </c>
       <c r="E8" s="8" t="s">
@@ -2994,7 +2990,7 @@
         <v>37</v>
       </c>
       <c r="L8" s="36" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="M8" s="37">
         <v>1352.9120938264666</v>
@@ -3005,15 +3001,15 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D9" s="44">
+        <v>79</v>
+      </c>
+      <c r="D9" s="41">
         <v>1345</v>
       </c>
       <c r="E9" s="8" t="s">
@@ -3039,21 +3035,21 @@
       </c>
       <c r="L9" s="36"/>
       <c r="M9" s="37" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="N9" s="38"/>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="D10" s="44">
+        <v>80</v>
+      </c>
+      <c r="D10" s="41">
         <v>264.01333542371003</v>
       </c>
       <c r="E10" s="8" t="s">
@@ -3078,26 +3074,26 @@
         <v>42</v>
       </c>
       <c r="L10" s="31" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="M10" s="19">
         <v>0</v>
       </c>
       <c r="N10" s="24" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="21" thickBot="1">
       <c r="A11" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="D11" s="44">
+        <v>81</v>
+      </c>
+      <c r="D11" s="41">
         <v>168.93444059755035</v>
       </c>
       <c r="E11" s="8" t="s">
@@ -3122,30 +3118,30 @@
         <v>44</v>
       </c>
       <c r="L11" s="31" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M11" s="19">
         <v>4.6957316168698044</v>
       </c>
       <c r="N11" s="24" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="21" thickBot="1">
       <c r="A12" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D12" s="47">
+        <v>78</v>
+      </c>
+      <c r="D12" s="44">
         <v>0</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>18</v>
@@ -3167,25 +3163,25 @@
       </c>
       <c r="L12" s="23"/>
       <c r="M12" s="32" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="N12" s="20"/>
     </row>
     <row r="13" spans="1:14" ht="21" thickBot="1">
       <c r="A13" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D13" s="44">
+        <v>79</v>
+      </c>
+      <c r="D13" s="41">
         <v>1.3929601241108407E-2</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>18</v>
@@ -3211,19 +3207,19 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="D14" s="45">
+        <v>77</v>
+      </c>
+      <c r="D14" s="42">
         <v>16.856278125343849</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>18</v>
@@ -3249,15 +3245,15 @@
     </row>
     <row r="15" spans="1:14" ht="21" thickBot="1">
       <c r="A15" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D15" s="46">
+        <v>78</v>
+      </c>
+      <c r="D15" s="43">
         <v>0</v>
       </c>
       <c r="E15" s="8" t="s">
@@ -3287,15 +3283,15 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D16" s="44">
+        <v>79</v>
+      </c>
+      <c r="D16" s="41">
         <v>2.3580759098686901</v>
       </c>
       <c r="E16" s="8" t="s">
@@ -3325,15 +3321,15 @@
     </row>
     <row r="17" spans="1:14">
       <c r="A17" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D17" s="48">
+        <v>80</v>
+      </c>
+      <c r="D17" s="45">
         <v>0.40666774884274093</v>
       </c>
       <c r="E17" s="10" t="s">

</xml_diff>